<commit_message>
excel course 1st course week 5
</commit_message>
<xml_diff>
--- a/Visualization/Excel Specialization/course 1/week 5/W05-V01-Print Preview.xlsx
+++ b/Visualization/Excel Specialization/course 1/week 5/W05-V01-Print Preview.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandeep Tukkunor\Desktop\100 Days Of Code\Visualization\Excel Specialization\course 1\week 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandeep Tukkunor\Desktop\100 Days Of Code\Visualization\Excel Specialization\course 1\Week 5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CAD0B7-D6F1-4ED7-8A18-DC4B621B0394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE00FA2-E139-4385-905C-75547AC31826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,12 +23,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -6011,7 +6005,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -6076,13 +6070,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="3" xfId="4" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Accent1" xfId="7" builtinId="29"/>
@@ -89918,21 +89905,20 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" style="29" customWidth="1"/>
-    <col min="3" max="5" width="13.77734375" customWidth="1"/>
+    <col min="2" max="5" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703" s="36" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>1912</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="37"/>
     </row>
     <row r="3" spans="1:703" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>865</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="16" t="s">
         <v>1913</v>
       </c>
       <c r="C3" s="16" t="s">
@@ -89949,7 +89935,7 @@
       <c r="A4" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4">
         <f>'Sales 2015'!F4</f>
         <v>3626.7196000000004</v>
       </c>
@@ -90015,7 +90001,7 @@
       <c r="A7" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="12">
         <f>'Sales 2015'!F7</f>
         <v>40848.891499999998</v>
       </c>
@@ -90036,7 +90022,7 @@
       <c r="A8" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="12">
         <f>'Sales 2015'!F8</f>
         <v>66900.426800000001</v>
       </c>
@@ -90057,7 +90043,7 @@
       <c r="A9" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="12">
         <f>'Sales 2015'!F9</f>
         <v>21231.873699999996</v>
       </c>
@@ -90078,7 +90064,7 @@
       <c r="A10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="12">
         <f>'Sales 2015'!F10</f>
         <v>20874.7706</v>
       </c>
@@ -90099,7 +90085,7 @@
       <c r="A11" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="12">
         <f>'Sales 2015'!F11</f>
         <v>22189.045700000002</v>
       </c>
@@ -90120,7 +90106,7 @@
       <c r="A12" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="12">
         <f>'Sales 2015'!F12</f>
         <v>6498.4348</v>
       </c>
@@ -90141,7 +90127,7 @@
       <c r="A13" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="12">
         <f>'Sales 2015'!F13</f>
         <v>21303.2778</v>
       </c>
@@ -90162,7 +90148,7 @@
       <c r="A14" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="12">
         <f>'Sales 2015'!F14</f>
         <v>39422.461900000002</v>
       </c>
@@ -90183,7 +90169,7 @@
       <c r="A15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="12">
         <f>'Sales 2015'!F15</f>
         <v>813.45619999999997</v>
       </c>
@@ -90204,7 +90190,7 @@
       <c r="A16" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="12">
         <f>'Sales 2015'!F16</f>
         <v>26975.758499999996</v>
       </c>
@@ -90225,7 +90211,7 @@
       <c r="A17" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="12">
         <f>'Sales 2015'!F17</f>
         <v>35551.663699999997</v>
       </c>
@@ -90246,7 +90232,7 @@
       <c r="A18" s="13" t="s">
         <v>856</v>
       </c>
-      <c r="B18" s="42">
+      <c r="B18" s="14">
         <f>'Sales 2015'!F18</f>
         <v>361480.79389999999</v>
       </c>

</xml_diff>